<commit_message>
record deleted for testing
</commit_message>
<xml_diff>
--- a/Fusion/ETL/Customers/Common/HCM/WorkStructuresMigration/WorkStructure_IFTY_V1_FUSN_R7/data-in/InfovityHCMEmployeesV1.xlsx
+++ b/Fusion/ETL/Customers/Common/HCM/WorkStructuresMigration/WorkStructure_IFTY_V1_FUSN_R7/data-in/InfovityHCMEmployeesV1.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="369">
   <si>
     <t>Regular or Temporary</t>
   </si>
@@ -1157,9 +1157,6 @@
   </si>
   <si>
     <t>Address Line 23</t>
-  </si>
-  <si>
-    <t>Address Line 24</t>
   </si>
   <si>
     <t>UK</t>
@@ -4620,9 +4617,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4813,7 +4810,7 @@
         <v>166</v>
       </c>
       <c r="N5" s="72" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="52" customFormat="1">
@@ -4855,7 +4852,7 @@
         <v>166</v>
       </c>
       <c r="N6" s="72" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="52" customFormat="1">
@@ -4897,7 +4894,7 @@
         <v>166</v>
       </c>
       <c r="N7" s="72" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="52" customFormat="1">
@@ -4939,7 +4936,7 @@
         <v>166</v>
       </c>
       <c r="N8" s="72" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="52" customFormat="1">
@@ -4981,7 +4978,7 @@
         <v>166</v>
       </c>
       <c r="N9" s="72" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="52" customFormat="1">
@@ -5023,7 +5020,7 @@
         <v>166</v>
       </c>
       <c r="N10" s="72" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="52" customFormat="1">
@@ -5065,7 +5062,7 @@
         <v>166</v>
       </c>
       <c r="N11" s="72" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="52" customFormat="1">
@@ -5107,7 +5104,7 @@
         <v>166</v>
       </c>
       <c r="N12" s="72" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="52" customFormat="1">
@@ -5149,7 +5146,7 @@
         <v>166</v>
       </c>
       <c r="N13" s="72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="52" customFormat="1">
@@ -5191,7 +5188,7 @@
         <v>166</v>
       </c>
       <c r="N14" s="72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="52" customFormat="1">
@@ -5231,7 +5228,7 @@
         <v>166</v>
       </c>
       <c r="N15" s="72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="52" customFormat="1">
@@ -5271,7 +5268,7 @@
         <v>166</v>
       </c>
       <c r="N16" s="72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="52" customFormat="1">
@@ -5311,7 +5308,7 @@
         <v>166</v>
       </c>
       <c r="N17" s="72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="52" customFormat="1">
@@ -5351,7 +5348,7 @@
         <v>166</v>
       </c>
       <c r="N18" s="72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="52" customFormat="1">
@@ -5391,7 +5388,7 @@
         <v>166</v>
       </c>
       <c r="N19" s="72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="52" customFormat="1">
@@ -5431,7 +5428,7 @@
         <v>166</v>
       </c>
       <c r="N20" s="72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="52" customFormat="1">
@@ -5471,48 +5468,24 @@
         <v>166</v>
       </c>
       <c r="N21" s="72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="52" customFormat="1">
       <c r="A22" s="72"/>
-      <c r="B22" s="73">
-        <v>40350</v>
-      </c>
+      <c r="B22" s="73"/>
       <c r="C22" s="69"/>
-      <c r="D22" s="69" t="s">
-        <v>168</v>
-      </c>
-      <c r="E22" s="72" t="s">
-        <v>163</v>
-      </c>
-      <c r="F22" s="72" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="72" t="s">
-        <v>366</v>
-      </c>
-      <c r="I22" s="72" t="s">
-        <v>164</v>
-      </c>
-      <c r="J22" s="72" t="s">
-        <v>165</v>
-      </c>
-      <c r="K22" s="72">
-        <v>49895</v>
-      </c>
-      <c r="L22" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="M22" s="71" t="s">
-        <v>166</v>
-      </c>
-      <c r="N22" s="72" t="s">
-        <v>367</v>
-      </c>
+      <c r="D22" s="69"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="71"/>
+      <c r="N22" s="72"/>
     </row>
     <row r="23" spans="1:14" s="52" customFormat="1">
       <c r="E23" s="53"/>

</xml_diff>